<commit_message>
modified rsast vs other method
</commit_message>
<xml_diff>
--- a/ExperimentationRSAST/DataSetsUCLASummary.xlsx
+++ b/ExperimentationRSAST/DataSetsUCLASummary.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="386">
   <si>
     <t>USED SAST</t>
   </si>
@@ -47,12 +47,12 @@
     <t>ID</t>
   </si>
   <si>
+    <t>Name</t>
+  </si>
+  <si>
     <t>Type</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t xml:space="preserve">Train </t>
   </si>
   <si>
@@ -83,36 +83,36 @@
     <t>Y</t>
   </si>
   <si>
+    <t>SmoothSubspace</t>
+  </si>
+  <si>
     <t>Simulated</t>
   </si>
   <si>
-    <t>SmoothSubspace</t>
-  </si>
-  <si>
     <t>0.0533 (1)</t>
   </si>
   <si>
     <t>X. Huang</t>
   </si>
   <si>
+    <t>Chinatown</t>
+  </si>
+  <si>
     <t>Traffic</t>
   </si>
   <si>
-    <t>Chinatown</t>
-  </si>
-  <si>
     <t>0.0466 (0)</t>
   </si>
   <si>
     <t>H.A. Dau</t>
   </si>
   <si>
+    <t>ItalyPowerDemand</t>
+  </si>
+  <si>
     <t>Sensor</t>
   </si>
   <si>
-    <t>ItalyPowerDemand</t>
-  </si>
-  <si>
     <t>0.0447 (0)</t>
   </si>
   <si>
@@ -131,12 +131,12 @@
     <t>With RidgeClassifier(alpha=10.0)</t>
   </si>
   <si>
+    <t>Crop</t>
+  </si>
+  <si>
     <t>Image</t>
   </si>
   <si>
-    <t>Crop</t>
-  </si>
-  <si>
     <t>0.2883 (0)</t>
   </si>
   <si>
@@ -233,12 +233,12 @@
     <t>0.2439 (2)</t>
   </si>
   <si>
+    <t>TwoLeadECG</t>
+  </si>
+  <si>
     <t>ECG</t>
   </si>
   <si>
-    <t>TwoLeadECG</t>
-  </si>
-  <si>
     <t>0.1317 (4)</t>
   </si>
   <si>
@@ -263,12 +263,12 @@
     <t>R. Olszewski</t>
   </si>
   <si>
+    <t>ElectricDevices</t>
+  </si>
+  <si>
     <t>Device</t>
   </si>
   <si>
-    <t>ElectricDevices</t>
-  </si>
-  <si>
     <t>0.3806 (14)</t>
   </si>
   <si>
@@ -362,24 +362,24 @@
     <t>J. Gao</t>
   </si>
   <si>
+    <t>PowerCons</t>
+  </si>
+  <si>
     <t>Power</t>
   </si>
   <si>
-    <t>PowerCons</t>
-  </si>
-  <si>
     <t>0.0778 (3)</t>
   </si>
   <si>
     <t>EDF R&amp;D, France</t>
   </si>
   <si>
+    <t>GunPoint</t>
+  </si>
+  <si>
     <t>Motion</t>
   </si>
   <si>
-    <t>GunPoint</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 0.0867 (0) </t>
   </si>
   <si>
@@ -434,24 +434,24 @@
     <t>A. Jalba</t>
   </si>
   <si>
+    <t>Fungi</t>
+  </si>
+  <si>
     <t>HRM</t>
   </si>
   <si>
-    <t>Fungi</t>
-  </si>
-  <si>
     <t>0.1774 (0)</t>
   </si>
   <si>
     <t>W. Fonzi</t>
   </si>
   <si>
+    <t>Wine</t>
+  </si>
+  <si>
     <t>Spectro</t>
   </si>
   <si>
-    <t>Wine</t>
-  </si>
-  <si>
     <t>0.3889 (0)</t>
   </si>
   <si>
@@ -755,12 +755,12 @@
     <t>0.2333 (1)</t>
   </si>
   <si>
+    <t>InsectEPGRegularTrain</t>
+  </si>
+  <si>
     <t>EPG</t>
   </si>
   <si>
-    <t>InsectEPGRegularTrain</t>
-  </si>
-  <si>
     <t>0.1727 (11)</t>
   </si>
   <si>
@@ -899,12 +899,12 @@
     <t>J. Brady</t>
   </si>
   <si>
+    <t>EOGHorizontalSignal</t>
+  </si>
+  <si>
     <t>EOG</t>
   </si>
   <si>
-    <t>EOGHorizontalSignal</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 0.5249 (1)</t>
   </si>
   <si>
@@ -926,12 +926,12 @@
     <t>P. Schafer</t>
   </si>
   <si>
+    <t>SemgHandGenderCh2</t>
+  </si>
+  <si>
     <t>Spectrum</t>
   </si>
   <si>
-    <t>SemgHandGenderCh2</t>
-  </si>
-  <si>
     <t>0.1550 (1)</t>
   </si>
   <si>
@@ -977,12 +977,12 @@
     <t xml:space="preserve"> 0.0588 (33)</t>
   </si>
   <si>
+    <t>PigAirwayPressure</t>
+  </si>
+  <si>
     <t>Hemodynamics</t>
   </si>
   <si>
-    <t>PigAirwayPressure</t>
-  </si>
-  <si>
     <t>0.9038 (1)</t>
   </si>
   <si>
@@ -1040,10 +1040,10 @@
     <t>0.3486 (11)</t>
   </si>
   <si>
+    <t>GestureMidAirD1</t>
+  </si>
+  <si>
     <t>Trajectory</t>
-  </si>
-  <si>
-    <t>GestureMidAirD1</t>
   </si>
   <si>
     <t xml:space="preserve"> 0.3615 (5)</t>
@@ -1253,8 +1253,8 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="10" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1281,8 +1281,8 @@
     <xf borderId="1" fillId="2" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf borderId="1" fillId="2" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="2" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1520,8 +1520,8 @@
     <col customWidth="1" min="7" max="7" width="11.14"/>
     <col customWidth="1" min="8" max="8" width="11.29"/>
     <col customWidth="1" min="9" max="9" width="5.86"/>
-    <col customWidth="1" min="10" max="10" width="14.29"/>
-    <col customWidth="1" min="11" max="11" width="30.86"/>
+    <col customWidth="1" min="10" max="10" width="30.86"/>
+    <col customWidth="1" min="11" max="11" width="14.29"/>
     <col customWidth="1" min="12" max="13" width="8.86"/>
     <col customWidth="1" min="14" max="14" width="9.43"/>
     <col customWidth="1" min="15" max="15" width="8.86"/>
@@ -1567,10 +1567,10 @@
       <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
       <c r="N1" s="6" t="s">
@@ -1621,16 +1621,16 @@
       <c r="I2" s="2">
         <v>127.0</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="5">
+      <c r="L2" s="4">
         <v>150.0</v>
       </c>
-      <c r="M2" s="5">
+      <c r="M2" s="4">
         <v>150.0</v>
       </c>
       <c r="N2" s="2">
@@ -1681,10 +1681,10 @@
       <c r="I3" s="2">
         <v>91.0</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="K3" s="4" t="s">
         <v>26</v>
       </c>
       <c r="L3" s="1">
@@ -1741,16 +1741,16 @@
       <c r="I4" s="2">
         <v>38.0</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="K4" s="9" t="s">
+      <c r="K4" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="L4" s="5">
+      <c r="L4" s="4">
         <v>67.0</v>
       </c>
-      <c r="M4" s="5">
+      <c r="M4" s="4">
         <v>1029.0</v>
       </c>
       <c r="N4" s="6">
@@ -1797,11 +1797,11 @@
       <c r="I5" s="2">
         <v>113.0</v>
       </c>
-      <c r="J5" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K5" s="13" t="s">
+      <c r="J5" s="13" t="s">
         <v>34</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="L5" s="1">
         <v>1194.0</v>
@@ -1853,10 +1853,10 @@
       <c r="I6" s="2">
         <v>92.0</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="J6" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="K6" s="13" t="s">
+      <c r="K6" s="4" t="s">
         <v>38</v>
       </c>
       <c r="L6" s="1">
@@ -1911,16 +1911,16 @@
       <c r="I7" s="2">
         <v>70.0</v>
       </c>
-      <c r="J7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K7" s="9" t="s">
+      <c r="J7" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="L7" s="5">
+      <c r="K7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="L7" s="4">
         <v>300.0</v>
       </c>
-      <c r="M7" s="5">
+      <c r="M7" s="4">
         <v>300.0</v>
       </c>
       <c r="N7" s="6">
@@ -1969,16 +1969,16 @@
       <c r="I8" s="2">
         <v>65.0</v>
       </c>
-      <c r="J8" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K8" s="9" t="s">
+      <c r="J8" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="L8" s="5">
+      <c r="K8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L8" s="4">
         <v>27.0</v>
       </c>
-      <c r="M8" s="5">
+      <c r="M8" s="4">
         <v>953.0</v>
       </c>
       <c r="N8" s="6">
@@ -2027,16 +2027,16 @@
       <c r="I9" s="2">
         <v>64.0</v>
       </c>
-      <c r="J9" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K9" s="9" t="s">
+      <c r="J9" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="L9" s="5">
+      <c r="K9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L9" s="4">
         <v>20.0</v>
       </c>
-      <c r="M9" s="5">
+      <c r="M9" s="4">
         <v>601.0</v>
       </c>
       <c r="N9" s="6">
@@ -2066,8 +2066,12 @@
         <v>20</v>
       </c>
       <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
+      <c r="C10" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="12">
+        <v>3.0</v>
+      </c>
       <c r="E10" s="3"/>
       <c r="F10" s="2">
         <v>6.0</v>
@@ -2081,16 +2085,16 @@
       <c r="I10" s="2">
         <v>16.0</v>
       </c>
-      <c r="J10" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="K10" s="13" t="s">
+      <c r="J10" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="L10" s="5">
+      <c r="K10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L10" s="4">
         <v>400.0</v>
       </c>
-      <c r="M10" s="5">
+      <c r="M10" s="4">
         <v>139.0</v>
       </c>
       <c r="N10" s="6">
@@ -2120,8 +2124,12 @@
         <v>20</v>
       </c>
       <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="2"/>
+      <c r="C11" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="12">
+        <v>1.0</v>
+      </c>
       <c r="E11" s="3"/>
       <c r="F11" s="2">
         <v>6.0</v>
@@ -2135,16 +2143,16 @@
       <c r="I11" s="2">
         <v>17.0</v>
       </c>
-      <c r="J11" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="K11" s="13" t="s">
+      <c r="J11" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="L11" s="5">
+      <c r="K11" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L11" s="4">
         <v>600.0</v>
       </c>
-      <c r="M11" s="5">
+      <c r="M11" s="4">
         <v>276.0</v>
       </c>
       <c r="N11" s="6">
@@ -2189,16 +2197,16 @@
       <c r="I12" s="2">
         <v>18.0</v>
       </c>
-      <c r="J12" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="K12" s="13" t="s">
+      <c r="J12" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="L12" s="5">
+      <c r="K12" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L12" s="4">
         <v>400.0</v>
       </c>
-      <c r="M12" s="5">
+      <c r="M12" s="4">
         <v>139.0</v>
       </c>
       <c r="N12" s="6">
@@ -2243,16 +2251,16 @@
       <c r="I13" s="2">
         <v>45.0</v>
       </c>
-      <c r="J13" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="K13" s="13" t="s">
+      <c r="J13" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="L13" s="5">
+      <c r="K13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L13" s="4">
         <v>400.0</v>
       </c>
-      <c r="M13" s="5">
+      <c r="M13" s="4">
         <v>154.0</v>
       </c>
       <c r="N13" s="6">
@@ -2297,16 +2305,16 @@
       <c r="I14" s="2">
         <v>46.0</v>
       </c>
-      <c r="J14" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="K14" s="13" t="s">
+      <c r="J14" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="L14" s="5">
+      <c r="K14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L14" s="4">
         <v>600.0</v>
       </c>
-      <c r="M14" s="5">
+      <c r="M14" s="4">
         <v>291.0</v>
       </c>
       <c r="N14" s="6">
@@ -2353,16 +2361,16 @@
       <c r="I15" s="2">
         <v>47.0</v>
       </c>
-      <c r="J15" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="K15" s="13" t="s">
+      <c r="J15" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="L15" s="5">
+      <c r="K15" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L15" s="4">
         <v>399.0</v>
       </c>
-      <c r="M15" s="5">
+      <c r="M15" s="4">
         <v>154.0</v>
       </c>
       <c r="N15" s="6">
@@ -2407,16 +2415,16 @@
       <c r="I16" s="2">
         <v>53.0</v>
       </c>
-      <c r="J16" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="K16" s="13" t="s">
+      <c r="J16" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="L16" s="5">
+      <c r="K16" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L16" s="4">
         <v>1800.0</v>
       </c>
-      <c r="M16" s="5">
+      <c r="M16" s="4">
         <v>858.0</v>
       </c>
       <c r="N16" s="6">
@@ -2461,16 +2469,16 @@
       <c r="I17" s="2">
         <v>56.0</v>
       </c>
-      <c r="J17" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="K17" s="13" t="s">
+      <c r="J17" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="L17" s="5">
+      <c r="K17" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L17" s="4">
         <v>400.0</v>
       </c>
-      <c r="M17" s="5">
+      <c r="M17" s="4">
         <v>205.0</v>
       </c>
       <c r="N17" s="6">
@@ -2515,16 +2523,16 @@
       <c r="I18" s="2">
         <v>57.0</v>
       </c>
-      <c r="J18" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="K18" s="13" t="s">
+      <c r="J18" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="L18" s="5">
+      <c r="K18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L18" s="4">
         <v>600.0</v>
       </c>
-      <c r="M18" s="5">
+      <c r="M18" s="4">
         <v>291.0</v>
       </c>
       <c r="N18" s="6">
@@ -2569,16 +2577,16 @@
       <c r="I19" s="2">
         <v>58.0</v>
       </c>
-      <c r="J19" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="K19" s="13" t="s">
+      <c r="J19" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="L19" s="5">
+      <c r="K19" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L19" s="4">
         <v>400.0</v>
       </c>
-      <c r="M19" s="5">
+      <c r="M19" s="4">
         <v>205.0</v>
       </c>
       <c r="N19" s="6">
@@ -2625,16 +2633,16 @@
       <c r="I20" s="2">
         <v>74.0</v>
       </c>
-      <c r="J20" s="5" t="s">
+      <c r="J20" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="K20" s="9" t="s">
+      <c r="K20" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="L20" s="5">
+      <c r="L20" s="4">
         <v>23.0</v>
       </c>
-      <c r="M20" s="5">
+      <c r="M20" s="4">
         <v>1139.0</v>
       </c>
       <c r="N20" s="6">
@@ -2681,16 +2689,16 @@
       <c r="I21" s="2">
         <v>48.0</v>
       </c>
-      <c r="J21" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K21" s="9" t="s">
+      <c r="J21" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="L21" s="5">
+      <c r="K21" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L21" s="4">
         <v>20.0</v>
       </c>
-      <c r="M21" s="5">
+      <c r="M21" s="4">
         <v>1252.0</v>
       </c>
       <c r="N21" s="6">
@@ -2737,16 +2745,16 @@
       <c r="I22" s="2">
         <v>20.0</v>
       </c>
-      <c r="J22" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="K22" s="9" t="s">
+      <c r="J22" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="L22" s="5">
+      <c r="K22" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="L22" s="4">
         <v>100.0</v>
       </c>
-      <c r="M22" s="5">
+      <c r="M22" s="4">
         <v>100.0</v>
       </c>
       <c r="N22" s="6">
@@ -2767,7 +2775,7 @@
       <c r="S22" s="10">
         <v>0.36</v>
       </c>
-      <c r="T22" s="5" t="s">
+      <c r="T22" s="4" t="s">
         <v>80</v>
       </c>
     </row>
@@ -2793,10 +2801,10 @@
       <c r="I23" s="2">
         <v>23.0</v>
       </c>
-      <c r="J23" s="5" t="s">
+      <c r="J23" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="K23" s="13" t="s">
+      <c r="K23" s="4" t="s">
         <v>82</v>
       </c>
       <c r="L23" s="1">
@@ -2849,16 +2857,16 @@
       <c r="I24" s="2">
         <v>44.0</v>
       </c>
-      <c r="J24" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="K24" s="9" t="s">
+      <c r="J24" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="L24" s="5">
+      <c r="K24" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L24" s="4">
         <v>381.0</v>
       </c>
-      <c r="M24" s="5">
+      <c r="M24" s="4">
         <v>760.0</v>
       </c>
       <c r="N24" s="6">
@@ -2903,16 +2911,16 @@
       <c r="I25" s="2">
         <v>90.0</v>
       </c>
-      <c r="J25" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K25" s="13" t="s">
+      <c r="J25" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="L25" s="5">
+      <c r="K25" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="L25" s="4">
         <v>30.0</v>
       </c>
-      <c r="M25" s="5">
+      <c r="M25" s="4">
         <v>150.0</v>
       </c>
       <c r="N25" s="2">
@@ -2933,7 +2941,7 @@
       <c r="S25" s="10">
         <v>0.6667</v>
       </c>
-      <c r="T25" s="5" t="s">
+      <c r="T25" s="4" t="s">
         <v>90</v>
       </c>
     </row>
@@ -2959,16 +2967,16 @@
       <c r="I26" s="2">
         <v>7.0</v>
       </c>
-      <c r="J26" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K26" s="9" t="s">
+      <c r="J26" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="L26" s="5">
+      <c r="K26" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="L26" s="4">
         <v>30.0</v>
       </c>
-      <c r="M26" s="5">
+      <c r="M26" s="4">
         <v>900.0</v>
       </c>
       <c r="N26" s="6">
@@ -3015,16 +3023,16 @@
       <c r="I27" s="2">
         <v>68.0</v>
       </c>
-      <c r="J27" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="K27" s="9" t="s">
+      <c r="J27" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="L27" s="5">
+      <c r="K27" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L27" s="4">
         <v>500.0</v>
       </c>
-      <c r="M27" s="5">
+      <c r="M27" s="4">
         <v>625.0</v>
       </c>
       <c r="N27" s="6">
@@ -3071,16 +3079,16 @@
       <c r="I28" s="2">
         <v>75.0</v>
       </c>
-      <c r="J28" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K28" s="9" t="s">
+      <c r="J28" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="L28" s="5">
+      <c r="K28" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="L28" s="4">
         <v>1000.0</v>
       </c>
-      <c r="M28" s="5">
+      <c r="M28" s="4">
         <v>4000.0</v>
       </c>
       <c r="N28" s="6">
@@ -3127,16 +3135,16 @@
       <c r="I29" s="2">
         <v>24.0</v>
       </c>
-      <c r="J29" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="K29" s="9" t="s">
+      <c r="J29" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="L29" s="5">
+      <c r="K29" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L29" s="4">
         <v>560.0</v>
       </c>
-      <c r="M29" s="5">
+      <c r="M29" s="4">
         <v>1690.0</v>
       </c>
       <c r="N29" s="6">
@@ -3183,16 +3191,16 @@
       <c r="I30" s="2">
         <v>26.0</v>
       </c>
-      <c r="J30" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="K30" s="9" t="s">
+      <c r="J30" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="L30" s="5">
+      <c r="K30" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L30" s="4">
         <v>200.0</v>
       </c>
-      <c r="M30" s="5">
+      <c r="M30" s="4">
         <v>2050.0</v>
       </c>
       <c r="N30" s="6">
@@ -3239,16 +3247,16 @@
       <c r="I31" s="2">
         <v>22.0</v>
       </c>
-      <c r="J31" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="K31" s="9" t="s">
+      <c r="J31" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="L31" s="5">
+      <c r="K31" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="L31" s="4">
         <v>23.0</v>
       </c>
-      <c r="M31" s="5">
+      <c r="M31" s="4">
         <v>861.0</v>
       </c>
       <c r="N31" s="6">
@@ -3295,16 +3303,16 @@
       <c r="I32" s="2">
         <v>21.0</v>
       </c>
-      <c r="J32" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="K32" s="9" t="s">
+      <c r="J32" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="L32" s="5">
+      <c r="K32" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="L32" s="4">
         <v>500.0</v>
       </c>
-      <c r="M32" s="5">
+      <c r="M32" s="4">
         <v>4500.0</v>
       </c>
       <c r="N32" s="6">
@@ -3351,16 +3359,16 @@
       <c r="I33" s="2">
         <v>55.0</v>
       </c>
-      <c r="J33" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K33" s="9" t="s">
+      <c r="J33" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="L33" s="5">
+      <c r="K33" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L33" s="4">
         <v>105.0</v>
       </c>
-      <c r="M33" s="5">
+      <c r="M33" s="4">
         <v>105.0</v>
       </c>
       <c r="N33" s="6">
@@ -3405,16 +3413,16 @@
       <c r="I34" s="2">
         <v>121.0</v>
       </c>
-      <c r="J34" s="5" t="s">
+      <c r="J34" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="K34" s="13" t="s">
+      <c r="K34" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="L34" s="5">
+      <c r="L34" s="4">
         <v>180.0</v>
       </c>
-      <c r="M34" s="5">
+      <c r="M34" s="4">
         <v>180.0</v>
       </c>
       <c r="N34" s="2">
@@ -3465,16 +3473,16 @@
       <c r="I35" s="2">
         <v>31.0</v>
       </c>
-      <c r="J35" s="5" t="s">
+      <c r="J35" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="K35" s="9" t="s">
+      <c r="K35" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="L35" s="5">
+      <c r="L35" s="4">
         <v>50.0</v>
       </c>
-      <c r="M35" s="5">
+      <c r="M35" s="4">
         <v>150.0</v>
       </c>
       <c r="N35" s="6">
@@ -3495,7 +3503,7 @@
       <c r="S35" s="10">
         <v>0.49333</v>
       </c>
-      <c r="T35" s="5" t="s">
+      <c r="T35" s="4" t="s">
         <v>121</v>
       </c>
     </row>
@@ -3519,16 +3527,16 @@
       <c r="I36" s="2">
         <v>107.0</v>
       </c>
-      <c r="J36" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="K36" s="13" t="s">
+      <c r="J36" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="L36" s="5">
+      <c r="K36" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="L36" s="4">
         <v>135.0</v>
       </c>
-      <c r="M36" s="5">
+      <c r="M36" s="4">
         <v>316.0</v>
       </c>
       <c r="N36" s="2">
@@ -3549,7 +3557,7 @@
       <c r="S36" s="10">
         <v>0.4937</v>
       </c>
-      <c r="T36" s="5" t="s">
+      <c r="T36" s="4" t="s">
         <v>121</v>
       </c>
     </row>
@@ -3573,16 +3581,16 @@
       <c r="I37" s="2">
         <v>108.0</v>
       </c>
-      <c r="J37" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="K37" s="13" t="s">
+      <c r="J37" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="L37" s="5">
+      <c r="K37" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="L37" s="4">
         <v>135.0</v>
       </c>
-      <c r="M37" s="5">
+      <c r="M37" s="4">
         <v>316.0</v>
       </c>
       <c r="N37" s="2">
@@ -3627,16 +3635,16 @@
       <c r="I38" s="2">
         <v>109.0</v>
       </c>
-      <c r="J38" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="K38" s="13" t="s">
+      <c r="J38" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="L38" s="5">
+      <c r="K38" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="L38" s="4">
         <v>136.0</v>
       </c>
-      <c r="M38" s="5">
+      <c r="M38" s="4">
         <v>315.0</v>
       </c>
       <c r="N38" s="2">
@@ -3681,16 +3689,16 @@
       <c r="I39" s="2">
         <v>128.0</v>
       </c>
-      <c r="J39" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K39" s="13" t="s">
+      <c r="J39" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="L39" s="5">
+      <c r="K39" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="L39" s="4">
         <v>36.0</v>
       </c>
-      <c r="M39" s="5">
+      <c r="M39" s="4">
         <v>144.0</v>
       </c>
       <c r="N39" s="2">
@@ -3737,16 +3745,16 @@
       <c r="I40" s="2">
         <v>80.0</v>
       </c>
-      <c r="J40" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K40" s="9" t="s">
+      <c r="J40" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="L40" s="5">
+      <c r="K40" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L40" s="4">
         <v>1000.0</v>
       </c>
-      <c r="M40" s="5">
+      <c r="M40" s="4">
         <v>6164.0</v>
       </c>
       <c r="N40" s="6">
@@ -3791,16 +3799,16 @@
       <c r="I41" s="2">
         <v>8.0</v>
       </c>
-      <c r="J41" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K41" s="9" t="s">
+      <c r="J41" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="L41" s="5">
+      <c r="K41" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L41" s="4">
         <v>467.0</v>
       </c>
-      <c r="M41" s="5">
+      <c r="M41" s="4">
         <v>3840.0</v>
       </c>
       <c r="N41" s="6">
@@ -3847,16 +3855,16 @@
       <c r="I42" s="2">
         <v>1.0</v>
       </c>
-      <c r="J42" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="K42" s="9" t="s">
+      <c r="J42" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="L42" s="5">
+      <c r="K42" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L42" s="4">
         <v>390.0</v>
       </c>
-      <c r="M42" s="5">
+      <c r="M42" s="4">
         <v>391.0</v>
       </c>
       <c r="N42" s="6">
@@ -3903,16 +3911,16 @@
       <c r="I43" s="2">
         <v>101.0</v>
       </c>
-      <c r="J43" s="5" t="s">
+      <c r="J43" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="K43" s="13" t="s">
+      <c r="K43" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="L43" s="5">
+      <c r="L43" s="4">
         <v>18.0</v>
       </c>
-      <c r="M43" s="5">
+      <c r="M43" s="4">
         <v>186.0</v>
       </c>
       <c r="N43" s="2">
@@ -3959,16 +3967,16 @@
       <c r="I44" s="2">
         <v>81.0</v>
       </c>
-      <c r="J44" s="5" t="s">
+      <c r="J44" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="K44" s="13" t="s">
+      <c r="K44" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="L44" s="5">
+      <c r="L44" s="4">
         <v>57.0</v>
       </c>
-      <c r="M44" s="5">
+      <c r="M44" s="4">
         <v>54.0</v>
       </c>
       <c r="N44" s="6">
@@ -4015,16 +4023,16 @@
       <c r="I45" s="2">
         <v>67.0</v>
       </c>
-      <c r="J45" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="K45" s="13" t="s">
+      <c r="J45" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="L45" s="5">
+      <c r="K45" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="L45" s="4">
         <v>613.0</v>
       </c>
-      <c r="M45" s="5">
+      <c r="M45" s="4">
         <v>370.0</v>
       </c>
       <c r="N45" s="6">
@@ -4071,16 +4079,16 @@
       <c r="I46" s="2">
         <v>2.0</v>
       </c>
-      <c r="J46" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="K46" s="9" t="s">
+      <c r="J46" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="L46" s="5">
+      <c r="K46" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L46" s="4">
         <v>36.0</v>
       </c>
-      <c r="M46" s="5">
+      <c r="M46" s="4">
         <v>175.0</v>
       </c>
       <c r="N46" s="6">
@@ -4125,11 +4133,11 @@
       <c r="I47" s="2">
         <v>37.0</v>
       </c>
-      <c r="J47" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K47" s="13" t="s">
+      <c r="J47" s="13" t="s">
         <v>151</v>
+      </c>
+      <c r="K47" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="L47" s="1">
         <v>220.0</v>
@@ -4181,16 +4189,16 @@
       <c r="I48" s="2">
         <v>27.0</v>
       </c>
-      <c r="J48" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="K48" s="9" t="s">
+      <c r="J48" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="L48" s="5">
+      <c r="K48" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L48" s="4">
         <v>450.0</v>
       </c>
-      <c r="M48" s="5">
+      <c r="M48" s="4">
         <v>455.0</v>
       </c>
       <c r="N48" s="6">
@@ -4237,16 +4245,16 @@
       <c r="I49" s="2">
         <v>82.0</v>
       </c>
-      <c r="J49" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="K49" s="9" t="s">
+      <c r="J49" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="L49" s="5">
+      <c r="K49" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L49" s="4">
         <v>267.0</v>
       </c>
-      <c r="M49" s="5">
+      <c r="M49" s="4">
         <v>638.0</v>
       </c>
       <c r="N49" s="6">
@@ -4293,16 +4301,16 @@
       <c r="I50" s="2">
         <v>73.0</v>
       </c>
-      <c r="J50" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K50" s="9" t="s">
+      <c r="J50" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="L50" s="5">
+      <c r="K50" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L50" s="4">
         <v>100.0</v>
       </c>
-      <c r="M50" s="5">
+      <c r="M50" s="4">
         <v>100.0</v>
       </c>
       <c r="N50" s="6">
@@ -4347,16 +4355,16 @@
       <c r="I51" s="2">
         <v>71.0</v>
       </c>
-      <c r="J51" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="K51" s="9" t="s">
+      <c r="J51" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="L51" s="5">
+      <c r="K51" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="L51" s="4">
         <v>40.0</v>
       </c>
-      <c r="M51" s="5">
+      <c r="M51" s="4">
         <v>228.0</v>
       </c>
       <c r="N51" s="6">
@@ -4403,16 +4411,16 @@
       <c r="I52" s="2">
         <v>10.0</v>
       </c>
-      <c r="J52" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="K52" s="9" t="s">
+      <c r="J52" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="L52" s="5">
+      <c r="K52" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="L52" s="4">
         <v>28.0</v>
       </c>
-      <c r="M52" s="5">
+      <c r="M52" s="4">
         <v>28.0</v>
       </c>
       <c r="N52" s="6">
@@ -4457,11 +4465,11 @@
       <c r="I53" s="2">
         <v>93.0</v>
       </c>
-      <c r="J53" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K53" s="13" t="s">
+      <c r="J53" s="13" t="s">
         <v>167</v>
+      </c>
+      <c r="K53" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="L53" s="1">
         <v>78.0</v>
@@ -4511,11 +4519,11 @@
       <c r="I54" s="2">
         <v>94.0</v>
       </c>
-      <c r="J54" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K54" s="13" t="s">
+      <c r="J54" s="13" t="s">
         <v>170</v>
+      </c>
+      <c r="K54" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="L54" s="1">
         <v>20.0</v>
@@ -4565,11 +4573,11 @@
       <c r="I55" s="2">
         <v>95.0</v>
       </c>
-      <c r="J55" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K55" s="13" t="s">
+      <c r="J55" s="13" t="s">
         <v>172</v>
+      </c>
+      <c r="K55" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="L55" s="1">
         <v>20.0</v>
@@ -4621,16 +4629,16 @@
       <c r="I56" s="2">
         <v>12.0</v>
       </c>
-      <c r="J56" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="K56" s="9" t="s">
+      <c r="J56" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="L56" s="5">
+      <c r="K56" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="L56" s="4">
         <v>390.0</v>
       </c>
-      <c r="M56" s="5">
+      <c r="M56" s="4">
         <v>390.0</v>
       </c>
       <c r="N56" s="6">
@@ -4677,16 +4685,16 @@
       <c r="I57" s="2">
         <v>13.0</v>
       </c>
-      <c r="J57" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="K57" s="9" t="s">
+      <c r="J57" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="L57" s="5">
+      <c r="K57" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="L57" s="4">
         <v>390.0</v>
       </c>
-      <c r="M57" s="5">
+      <c r="M57" s="4">
         <v>390.0</v>
       </c>
       <c r="N57" s="6">
@@ -4733,16 +4741,16 @@
       <c r="I58" s="2">
         <v>14.0</v>
       </c>
-      <c r="J58" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="K58" s="9" t="s">
+      <c r="J58" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="L58" s="5">
+      <c r="K58" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="L58" s="4">
         <v>390.0</v>
       </c>
-      <c r="M58" s="5">
+      <c r="M58" s="4">
         <v>390.0</v>
       </c>
       <c r="N58" s="6">
@@ -4787,16 +4795,16 @@
       <c r="I59" s="2">
         <v>99.0</v>
       </c>
-      <c r="J59" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K59" s="13" t="s">
+      <c r="J59" s="13" t="s">
         <v>181</v>
       </c>
-      <c r="L59" s="5">
+      <c r="K59" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L59" s="4">
         <v>150.0</v>
       </c>
-      <c r="M59" s="5">
+      <c r="M59" s="4">
         <v>2850.0</v>
       </c>
       <c r="N59" s="2">
@@ -4841,16 +4849,16 @@
       <c r="I60" s="2">
         <v>100.0</v>
       </c>
-      <c r="J60" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K60" s="13" t="s">
+      <c r="J60" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="L60" s="5">
+      <c r="K60" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L60" s="4">
         <v>28.0</v>
       </c>
-      <c r="M60" s="5">
+      <c r="M60" s="4">
         <v>2850.0</v>
       </c>
       <c r="N60" s="2">
@@ -4884,16 +4892,16 @@
       <c r="I61" s="2">
         <v>77.0</v>
       </c>
-      <c r="J61" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="K61" s="9" t="s">
+      <c r="J61" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="L61" s="5">
+      <c r="K61" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="L61" s="4">
         <v>896.0</v>
       </c>
-      <c r="M61" s="5">
+      <c r="M61" s="4">
         <v>3582.0</v>
       </c>
       <c r="N61" s="6">
@@ -4927,16 +4935,16 @@
       <c r="I62" s="2">
         <v>78.0</v>
       </c>
-      <c r="J62" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="K62" s="9" t="s">
+      <c r="J62" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="L62" s="5">
+      <c r="K62" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="L62" s="4">
         <v>896.0</v>
       </c>
-      <c r="M62" s="5">
+      <c r="M62" s="4">
         <v>3582.0</v>
       </c>
       <c r="N62" s="6">
@@ -4970,16 +4978,16 @@
       <c r="I63" s="2">
         <v>79.0</v>
       </c>
-      <c r="J63" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="K63" s="9" t="s">
+      <c r="J63" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="L63" s="5">
+      <c r="K63" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="L63" s="4">
         <v>896.0</v>
       </c>
-      <c r="M63" s="5">
+      <c r="M63" s="4">
         <v>3582.0</v>
       </c>
       <c r="N63" s="6">
@@ -5016,16 +5024,16 @@
       <c r="I64" s="2">
         <v>41.0</v>
       </c>
-      <c r="J64" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K64" s="9" t="s">
+      <c r="J64" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="L64" s="5">
+      <c r="K64" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L64" s="4">
         <v>70.0</v>
       </c>
-      <c r="M64" s="5">
+      <c r="M64" s="4">
         <v>73.0</v>
       </c>
       <c r="N64" s="6">
@@ -5070,16 +5078,16 @@
       <c r="I65" s="2">
         <v>72.0</v>
       </c>
-      <c r="J65" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="K65" s="9" t="s">
+      <c r="J65" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="L65" s="5">
+      <c r="K65" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="L65" s="4">
         <v>36.0</v>
       </c>
-      <c r="M65" s="5">
+      <c r="M65" s="4">
         <v>130.0</v>
       </c>
       <c r="N65" s="6">
@@ -5124,16 +5132,16 @@
       <c r="I66" s="2">
         <v>15.0</v>
       </c>
-      <c r="J66" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="K66" s="9" t="s">
+      <c r="J66" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="L66" s="5">
+      <c r="K66" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L66" s="4">
         <v>16.0</v>
       </c>
-      <c r="M66" s="5">
+      <c r="M66" s="4">
         <v>306.0</v>
       </c>
       <c r="N66" s="6">
@@ -5154,7 +5162,7 @@
       <c r="S66" s="10">
         <v>0.69281</v>
       </c>
-      <c r="T66" s="5" t="s">
+      <c r="T66" s="4" t="s">
         <v>200</v>
       </c>
     </row>
@@ -5180,16 +5188,16 @@
       <c r="I67" s="2">
         <v>25.0</v>
       </c>
-      <c r="J67" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="K67" s="9" t="s">
+      <c r="J67" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="L67" s="5">
+      <c r="K67" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L67" s="4">
         <v>24.0</v>
       </c>
-      <c r="M67" s="5">
+      <c r="M67" s="4">
         <v>88.0</v>
       </c>
       <c r="N67" s="6">
@@ -5210,7 +5218,7 @@
       <c r="S67" s="10">
         <v>0.7045</v>
       </c>
-      <c r="T67" s="5" t="s">
+      <c r="T67" s="4" t="s">
         <v>121</v>
       </c>
     </row>
@@ -5236,16 +5244,16 @@
       <c r="I68" s="2">
         <v>69.0</v>
       </c>
-      <c r="J68" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="K68" s="9" t="s">
+      <c r="J68" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="L68" s="5">
+      <c r="K68" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L68" s="4">
         <v>25.0</v>
       </c>
-      <c r="M68" s="5">
+      <c r="M68" s="4">
         <v>995.0</v>
       </c>
       <c r="N68" s="6">
@@ -5282,16 +5290,16 @@
       <c r="I69" s="2">
         <v>85.0</v>
       </c>
-      <c r="J69" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="K69" s="9" t="s">
+      <c r="J69" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="L69" s="5">
+      <c r="K69" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L69" s="4">
         <v>300.0</v>
       </c>
-      <c r="M69" s="5">
+      <c r="M69" s="4">
         <v>3000.0</v>
       </c>
       <c r="N69" s="6">
@@ -5328,16 +5336,16 @@
       <c r="I70" s="2">
         <v>52.0</v>
       </c>
-      <c r="J70" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="K70" s="9" t="s">
+      <c r="J70" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="L70" s="5">
+      <c r="K70" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L70" s="4">
         <v>200.0</v>
       </c>
-      <c r="M70" s="5">
+      <c r="M70" s="4">
         <v>242.0</v>
       </c>
       <c r="N70" s="6">
@@ -5384,16 +5392,16 @@
       <c r="I71" s="2">
         <v>32.0</v>
       </c>
-      <c r="J71" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="K71" s="13" t="s">
+      <c r="J71" s="13" t="s">
         <v>212</v>
       </c>
-      <c r="L71" s="5">
+      <c r="K71" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="L71" s="4">
         <v>109.0</v>
       </c>
-      <c r="M71" s="5">
+      <c r="M71" s="4">
         <v>105.0</v>
       </c>
       <c r="N71" s="6">
@@ -5440,16 +5448,16 @@
       <c r="I72" s="2">
         <v>43.0</v>
       </c>
-      <c r="J72" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="K72" s="9" t="s">
+      <c r="J72" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="L72" s="5">
+      <c r="K72" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="L72" s="4">
         <v>60.0</v>
       </c>
-      <c r="M72" s="5">
+      <c r="M72" s="4">
         <v>60.0</v>
       </c>
       <c r="N72" s="6">
@@ -5486,16 +5494,16 @@
       <c r="I73" s="2">
         <v>28.0</v>
       </c>
-      <c r="J73" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="K73" s="9" t="s">
+      <c r="J73" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="L73" s="5">
+      <c r="K73" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L73" s="4">
         <v>175.0</v>
       </c>
-      <c r="M73" s="5">
+      <c r="M73" s="4">
         <v>175.0</v>
       </c>
       <c r="N73" s="6">
@@ -5542,16 +5550,16 @@
       <c r="I74" s="2">
         <v>3.0</v>
       </c>
-      <c r="J74" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="K74" s="9" t="s">
+      <c r="J74" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="L74" s="5">
+      <c r="K74" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="L74" s="4">
         <v>30.0</v>
       </c>
-      <c r="M74" s="5">
+      <c r="M74" s="4">
         <v>30.0</v>
       </c>
       <c r="N74" s="6">
@@ -5588,11 +5596,11 @@
       <c r="I75" s="2">
         <v>29.0</v>
       </c>
-      <c r="J75" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K75" s="13" t="s">
+      <c r="J75" s="13" t="s">
         <v>223</v>
+      </c>
+      <c r="K75" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="L75" s="1">
         <v>3601.0</v>
@@ -5634,16 +5642,16 @@
       <c r="I76" s="2">
         <v>30.0</v>
       </c>
-      <c r="J76" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K76" s="13" t="s">
+      <c r="J76" s="13" t="s">
         <v>225</v>
       </c>
-      <c r="L76" s="5">
+      <c r="K76" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L76" s="4">
         <v>3636.0</v>
       </c>
-      <c r="M76" s="5">
+      <c r="M76" s="4">
         <v>810.0</v>
       </c>
       <c r="N76" s="6">
@@ -5694,16 +5702,16 @@
       <c r="I77" s="2">
         <v>61.0</v>
       </c>
-      <c r="J77" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K77" s="9" t="s">
+      <c r="J77" s="9" t="s">
         <v>227</v>
       </c>
-      <c r="L77" s="5">
+      <c r="K77" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="L77" s="4">
         <v>20.0</v>
       </c>
-      <c r="M77" s="5">
+      <c r="M77" s="4">
         <v>180.0</v>
       </c>
       <c r="N77" s="6">
@@ -5740,16 +5748,16 @@
       <c r="I78" s="2">
         <v>62.0</v>
       </c>
-      <c r="J78" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="K78" s="9" t="s">
+      <c r="J78" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="L78" s="5">
+      <c r="K78" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L78" s="4">
         <v>600.0</v>
       </c>
-      <c r="M78" s="5">
+      <c r="M78" s="4">
         <v>600.0</v>
       </c>
       <c r="N78" s="6">
@@ -5796,16 +5804,16 @@
       <c r="I79" s="2">
         <v>4.0</v>
       </c>
-      <c r="J79" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="K79" s="13" t="s">
+      <c r="J79" s="13" t="s">
         <v>232</v>
       </c>
-      <c r="L79" s="5">
+      <c r="K79" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L79" s="4">
         <v>20.0</v>
       </c>
-      <c r="M79" s="5">
+      <c r="M79" s="4">
         <v>20.0</v>
       </c>
       <c r="N79" s="6">
@@ -5858,16 +5866,16 @@
       <c r="I80" s="2">
         <v>5.0</v>
       </c>
-      <c r="J80" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="K80" s="9" t="s">
+      <c r="J80" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="L80" s="5">
+      <c r="K80" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L80" s="4">
         <v>20.0</v>
       </c>
-      <c r="M80" s="5">
+      <c r="M80" s="4">
         <v>20.0</v>
       </c>
       <c r="N80" s="6">
@@ -5914,16 +5922,16 @@
       <c r="I81" s="2">
         <v>19.0</v>
       </c>
-      <c r="J81" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K81" s="13" t="s">
+      <c r="J81" s="13" t="s">
         <v>236</v>
       </c>
-      <c r="L81" s="5">
+      <c r="K81" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L81" s="4">
         <v>322.0</v>
       </c>
-      <c r="M81" s="5">
+      <c r="M81" s="4">
         <v>139.0</v>
       </c>
       <c r="N81" s="6">
@@ -5970,16 +5978,16 @@
       <c r="I82" s="2">
         <v>35.0</v>
       </c>
-      <c r="J82" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="K82" s="9" t="s">
+      <c r="J82" s="9" t="s">
         <v>238</v>
       </c>
-      <c r="L82" s="5">
+      <c r="K82" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L82" s="4">
         <v>64.0</v>
       </c>
-      <c r="M82" s="5">
+      <c r="M82" s="4">
         <v>64.0</v>
       </c>
       <c r="N82" s="6">
@@ -6016,16 +6024,16 @@
       <c r="I83" s="2">
         <v>51.0</v>
       </c>
-      <c r="J83" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="K83" s="9" t="s">
+      <c r="J83" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="L83" s="5">
+      <c r="K83" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="L83" s="4">
         <v>30.0</v>
       </c>
-      <c r="M83" s="5">
+      <c r="M83" s="4">
         <v>30.0</v>
       </c>
       <c r="N83" s="6">
@@ -6072,16 +6080,16 @@
       <c r="I84" s="2">
         <v>6.0</v>
       </c>
-      <c r="J84" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K84" s="9" t="s">
+      <c r="J84" s="9" t="s">
         <v>243</v>
       </c>
-      <c r="L84" s="5">
+      <c r="K84" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L84" s="4">
         <v>60.0</v>
       </c>
-      <c r="M84" s="5">
+      <c r="M84" s="4">
         <v>60.0</v>
       </c>
       <c r="N84" s="6">
@@ -6115,16 +6123,16 @@
       <c r="I85" s="2">
         <v>111.0</v>
       </c>
-      <c r="J85" s="5" t="s">
+      <c r="J85" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="K85" s="13" t="s">
+      <c r="K85" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="L85" s="5">
+      <c r="L85" s="4">
         <v>62.0</v>
       </c>
-      <c r="M85" s="5">
+      <c r="M85" s="4">
         <v>249.0</v>
       </c>
       <c r="N85" s="2">
@@ -6158,16 +6166,16 @@
       <c r="I86" s="2">
         <v>112.0</v>
       </c>
-      <c r="J86" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="K86" s="13" t="s">
+      <c r="J86" s="13" t="s">
         <v>249</v>
       </c>
-      <c r="L86" s="5">
+      <c r="K86" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="L86" s="4">
         <v>17.0</v>
       </c>
-      <c r="M86" s="5">
+      <c r="M86" s="4">
         <v>249.0</v>
       </c>
       <c r="N86" s="2">
@@ -6204,16 +6212,16 @@
       <c r="I87" s="2">
         <v>40.0</v>
       </c>
-      <c r="J87" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K87" s="9" t="s">
+      <c r="J87" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="L87" s="5">
+      <c r="K87" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L87" s="4">
         <v>60.0</v>
       </c>
-      <c r="M87" s="5">
+      <c r="M87" s="4">
         <v>61.0</v>
       </c>
       <c r="N87" s="6">
@@ -6250,16 +6258,16 @@
       <c r="I88" s="2">
         <v>11.0</v>
       </c>
-      <c r="J88" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="K88" s="9" t="s">
+      <c r="J88" s="9" t="s">
         <v>253</v>
       </c>
-      <c r="L88" s="5">
+      <c r="K88" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="L88" s="4">
         <v>250.0</v>
       </c>
-      <c r="M88" s="5">
+      <c r="M88" s="4">
         <v>250.0</v>
       </c>
       <c r="N88" s="6">
@@ -6293,16 +6301,16 @@
       <c r="I89" s="2">
         <v>39.0</v>
       </c>
-      <c r="J89" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="K89" s="9" t="s">
+      <c r="J89" s="9" t="s">
         <v>256</v>
       </c>
-      <c r="L89" s="5">
+      <c r="K89" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="L89" s="4">
         <v>375.0</v>
       </c>
-      <c r="M89" s="5">
+      <c r="M89" s="4">
         <v>375.0</v>
       </c>
       <c r="N89" s="6">
@@ -6336,16 +6344,16 @@
       <c r="I90" s="2">
         <v>59.0</v>
       </c>
-      <c r="J90" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="K90" s="9" t="s">
+      <c r="J90" s="9" t="s">
         <v>258</v>
       </c>
-      <c r="L90" s="5">
+      <c r="K90" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="L90" s="4">
         <v>375.0</v>
       </c>
-      <c r="M90" s="5">
+      <c r="M90" s="4">
         <v>375.0</v>
       </c>
       <c r="N90" s="6">
@@ -6382,16 +6390,16 @@
       <c r="I91" s="2">
         <v>60.0</v>
       </c>
-      <c r="J91" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="K91" s="9" t="s">
+      <c r="J91" s="9" t="s">
         <v>260</v>
       </c>
-      <c r="L91" s="5">
+      <c r="K91" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="L91" s="4">
         <v>375.0</v>
       </c>
-      <c r="M91" s="5">
+      <c r="M91" s="4">
         <v>375.0</v>
       </c>
       <c r="N91" s="6">
@@ -6425,16 +6433,16 @@
       <c r="I92" s="2">
         <v>63.0</v>
       </c>
-      <c r="J92" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="K92" s="9" t="s">
+      <c r="J92" s="9" t="s">
         <v>262</v>
       </c>
-      <c r="L92" s="5">
+      <c r="K92" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="L92" s="4">
         <v>375.0</v>
       </c>
-      <c r="M92" s="5">
+      <c r="M92" s="4">
         <v>375.0</v>
       </c>
       <c r="N92" s="6">
@@ -6468,11 +6476,11 @@
       <c r="I93" s="2">
         <v>49.0</v>
       </c>
-      <c r="J93" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="K93" s="13" t="s">
+      <c r="J93" s="13" t="s">
         <v>264</v>
+      </c>
+      <c r="K93" s="4" t="s">
+        <v>72</v>
       </c>
       <c r="L93" s="1">
         <v>1800.0</v>
@@ -6511,11 +6519,11 @@
       <c r="I94" s="2">
         <v>50.0</v>
       </c>
-      <c r="J94" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="K94" s="13" t="s">
+      <c r="J94" s="13" t="s">
         <v>267</v>
+      </c>
+      <c r="K94" s="4" t="s">
+        <v>72</v>
       </c>
       <c r="L94" s="1">
         <v>1800.0</v>
@@ -6557,16 +6565,16 @@
       <c r="I95" s="2">
         <v>83.0</v>
       </c>
-      <c r="J95" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="K95" s="13" t="s">
+      <c r="J95" s="13" t="s">
         <v>269</v>
       </c>
-      <c r="L95" s="5">
+      <c r="K95" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="L95" s="4">
         <v>181.0</v>
       </c>
-      <c r="M95" s="5">
+      <c r="M95" s="4">
         <v>77.0</v>
       </c>
       <c r="N95" s="6">
@@ -6603,16 +6611,16 @@
       <c r="I96" s="2">
         <v>84.0</v>
       </c>
-      <c r="J96" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="K96" s="13" t="s">
+      <c r="J96" s="13" t="s">
         <v>271</v>
       </c>
-      <c r="L96" s="5">
+      <c r="K96" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="L96" s="4">
         <v>181.0</v>
       </c>
-      <c r="M96" s="5">
+      <c r="M96" s="4">
         <v>77.0</v>
       </c>
       <c r="N96" s="6">
@@ -6646,16 +6654,16 @@
       <c r="I97" s="2">
         <v>76.0</v>
       </c>
-      <c r="J97" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="K97" s="9" t="s">
+      <c r="J97" s="9" t="s">
         <v>273</v>
       </c>
-      <c r="L97" s="5">
+      <c r="K97" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="L97" s="4">
         <v>896.0</v>
       </c>
-      <c r="M97" s="5">
+      <c r="M97" s="4">
         <v>3582.0</v>
       </c>
       <c r="N97" s="6">
@@ -6692,16 +6700,16 @@
       <c r="I98" s="2">
         <v>42.0</v>
       </c>
-      <c r="J98" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K98" s="9" t="s">
+      <c r="J98" s="9" t="s">
         <v>276</v>
       </c>
-      <c r="L98" s="5">
+      <c r="K98" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="L98" s="4">
         <v>55.0</v>
       </c>
-      <c r="M98" s="5">
+      <c r="M98" s="4">
         <v>2345.0</v>
       </c>
       <c r="N98" s="6">
@@ -6735,11 +6743,11 @@
       <c r="I99" s="2">
         <v>114.0</v>
       </c>
-      <c r="J99" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="K99" s="13" t="s">
+      <c r="J99" s="13" t="s">
         <v>279</v>
+      </c>
+      <c r="K99" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="L99" s="1">
         <v>500.0</v>
@@ -6778,11 +6786,11 @@
       <c r="I100" s="2">
         <v>115.0</v>
       </c>
-      <c r="J100" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="K100" s="13" t="s">
+      <c r="J100" s="13" t="s">
         <v>282</v>
+      </c>
+      <c r="K100" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="L100" s="1">
         <v>100.0</v>
@@ -6824,16 +6832,16 @@
       <c r="I101" s="2">
         <v>54.0</v>
       </c>
-      <c r="J101" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K101" s="9" t="s">
+      <c r="J101" s="9" t="s">
         <v>284</v>
       </c>
-      <c r="L101" s="5">
+      <c r="K101" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L101" s="4">
         <v>214.0</v>
       </c>
-      <c r="M101" s="5">
+      <c r="M101" s="4">
         <v>1896.0</v>
       </c>
       <c r="N101" s="6">
@@ -6870,11 +6878,11 @@
       <c r="I102" s="2">
         <v>66.0</v>
       </c>
-      <c r="J102" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K102" s="13" t="s">
+      <c r="J102" s="13" t="s">
         <v>287</v>
+      </c>
+      <c r="K102" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="L102" s="1">
         <v>1000.0</v>
@@ -6916,16 +6924,16 @@
       <c r="I103" s="2">
         <v>34.0</v>
       </c>
-      <c r="J103" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="K103" s="9" t="s">
+      <c r="J103" s="9" t="s">
         <v>290</v>
       </c>
-      <c r="L103" s="5">
+      <c r="K103" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="L103" s="4">
         <v>155.0</v>
       </c>
-      <c r="M103" s="5">
+      <c r="M103" s="4">
         <v>308.0</v>
       </c>
       <c r="N103" s="6">
@@ -6959,10 +6967,10 @@
       <c r="I104" s="2">
         <v>96.0</v>
       </c>
-      <c r="J104" s="5" t="s">
+      <c r="J104" s="13" t="s">
         <v>293</v>
       </c>
-      <c r="K104" s="13" t="s">
+      <c r="K104" s="4" t="s">
         <v>294</v>
       </c>
       <c r="L104" s="1">
@@ -7002,11 +7010,11 @@
       <c r="I105" s="2">
         <v>97.0</v>
       </c>
-      <c r="J105" s="5" t="s">
-        <v>293</v>
-      </c>
-      <c r="K105" s="13" t="s">
+      <c r="J105" s="13" t="s">
         <v>297</v>
+      </c>
+      <c r="K105" s="4" t="s">
+        <v>294</v>
       </c>
       <c r="L105" s="1">
         <v>362.0</v>
@@ -7046,15 +7054,15 @@
         <v>86.0</v>
       </c>
       <c r="J106" s="16" t="s">
-        <v>81</v>
+        <v>299</v>
       </c>
       <c r="K106" s="17" t="s">
-        <v>299</v>
-      </c>
-      <c r="L106" s="16">
+        <v>82</v>
+      </c>
+      <c r="L106" s="17">
         <v>100.0</v>
       </c>
-      <c r="M106" s="16">
+      <c r="M106" s="17">
         <v>100.0</v>
       </c>
       <c r="N106" s="14">
@@ -7088,10 +7096,10 @@
       <c r="I107" s="2">
         <v>123.0</v>
       </c>
-      <c r="J107" s="5" t="s">
+      <c r="J107" s="13" t="s">
         <v>302</v>
       </c>
-      <c r="K107" s="13" t="s">
+      <c r="K107" s="4" t="s">
         <v>303</v>
       </c>
       <c r="L107" s="1">
@@ -7131,11 +7139,11 @@
       <c r="I108" s="2">
         <v>124.0</v>
       </c>
-      <c r="J108" s="5" t="s">
-        <v>302</v>
-      </c>
-      <c r="K108" s="13" t="s">
+      <c r="J108" s="13" t="s">
         <v>305</v>
+      </c>
+      <c r="K108" s="4" t="s">
+        <v>303</v>
       </c>
       <c r="L108" s="1">
         <v>450.0</v>
@@ -7174,11 +7182,11 @@
       <c r="I109" s="2">
         <v>125.0</v>
       </c>
-      <c r="J109" s="5" t="s">
-        <v>302</v>
-      </c>
-      <c r="K109" s="13" t="s">
+      <c r="J109" s="13" t="s">
         <v>307</v>
+      </c>
+      <c r="K109" s="4" t="s">
+        <v>303</v>
       </c>
       <c r="L109" s="1">
         <v>450.0</v>
@@ -7220,16 +7228,16 @@
       <c r="I110" s="2">
         <v>9.0</v>
       </c>
-      <c r="J110" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K110" s="9" t="s">
+      <c r="J110" s="9" t="s">
         <v>309</v>
       </c>
-      <c r="L110" s="5">
+      <c r="K110" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L110" s="4">
         <v>40.0</v>
       </c>
-      <c r="M110" s="5">
+      <c r="M110" s="4">
         <v>1380.0</v>
       </c>
       <c r="N110" s="6">
@@ -7263,16 +7271,16 @@
       <c r="I111" s="2">
         <v>98.0</v>
       </c>
-      <c r="J111" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="K111" s="13" t="s">
+      <c r="J111" s="13" t="s">
         <v>312</v>
       </c>
-      <c r="L111" s="5">
+      <c r="K111" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="L111" s="4">
         <v>504.0</v>
       </c>
-      <c r="M111" s="5">
+      <c r="M111" s="4">
         <v>500.0</v>
       </c>
       <c r="N111" s="2">
@@ -7309,16 +7317,16 @@
       <c r="I112" s="2">
         <v>36.0</v>
       </c>
-      <c r="J112" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="K112" s="9" t="s">
+      <c r="J112" s="9" t="s">
         <v>314</v>
       </c>
-      <c r="L112" s="5">
+      <c r="K112" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="L112" s="4">
         <v>100.0</v>
       </c>
-      <c r="M112" s="5">
+      <c r="M112" s="4">
         <v>550.0</v>
       </c>
       <c r="N112" s="6">
@@ -7352,16 +7360,16 @@
       <c r="I113" s="2">
         <v>110.0</v>
       </c>
-      <c r="J113" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="K113" s="13" t="s">
+      <c r="J113" s="13" t="s">
         <v>317</v>
       </c>
-      <c r="L113" s="5">
+      <c r="K113" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="L113" s="4">
         <v>40.0</v>
       </c>
-      <c r="M113" s="5">
+      <c r="M113" s="4">
         <v>119.0</v>
       </c>
       <c r="N113" s="2">
@@ -7395,16 +7403,16 @@
       <c r="I114" s="2">
         <v>117.0</v>
       </c>
-      <c r="J114" s="5" t="s">
+      <c r="J114" s="13" t="s">
         <v>319</v>
       </c>
-      <c r="K114" s="13" t="s">
+      <c r="K114" s="4" t="s">
         <v>320</v>
       </c>
-      <c r="L114" s="5">
+      <c r="L114" s="4">
         <v>104.0</v>
       </c>
-      <c r="M114" s="5">
+      <c r="M114" s="4">
         <v>208.0</v>
       </c>
       <c r="N114" s="2">
@@ -7425,7 +7433,7 @@
       <c r="S114" s="10">
         <v>0.9808</v>
       </c>
-      <c r="T114" s="5" t="s">
+      <c r="T114" s="4" t="s">
         <v>322</v>
       </c>
     </row>
@@ -7438,16 +7446,16 @@
       <c r="I115" s="2">
         <v>118.0</v>
       </c>
-      <c r="J115" s="5" t="s">
-        <v>319</v>
-      </c>
-      <c r="K115" s="13" t="s">
+      <c r="J115" s="13" t="s">
         <v>323</v>
       </c>
-      <c r="L115" s="5">
+      <c r="K115" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="L115" s="4">
         <v>104.0</v>
       </c>
-      <c r="M115" s="5">
+      <c r="M115" s="4">
         <v>208.0</v>
       </c>
       <c r="N115" s="2">
@@ -7468,7 +7476,7 @@
       <c r="S115" s="10">
         <v>0.9808</v>
       </c>
-      <c r="T115" s="5" t="s">
+      <c r="T115" s="4" t="s">
         <v>322</v>
       </c>
     </row>
@@ -7481,16 +7489,16 @@
       <c r="I116" s="2">
         <v>119.0</v>
       </c>
-      <c r="J116" s="5" t="s">
-        <v>319</v>
-      </c>
-      <c r="K116" s="13" t="s">
+      <c r="J116" s="13" t="s">
         <v>325</v>
       </c>
-      <c r="L116" s="5">
+      <c r="K116" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="L116" s="4">
         <v>104.0</v>
       </c>
-      <c r="M116" s="5">
+      <c r="M116" s="4">
         <v>208.0</v>
       </c>
       <c r="N116" s="2">
@@ -7511,7 +7519,7 @@
       <c r="S116" s="10">
         <v>0.9808</v>
       </c>
-      <c r="T116" s="5" t="s">
+      <c r="T116" s="4" t="s">
         <v>322</v>
       </c>
     </row>
@@ -7527,11 +7535,11 @@
       <c r="I117" s="2">
         <v>33.0</v>
       </c>
-      <c r="J117" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="K117" s="13" t="s">
+      <c r="J117" s="13" t="s">
         <v>327</v>
+      </c>
+      <c r="K117" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="L117" s="1">
         <v>1000.0</v>
@@ -7570,11 +7578,11 @@
       <c r="I118" s="2">
         <v>122.0</v>
       </c>
-      <c r="J118" s="5" t="s">
-        <v>302</v>
-      </c>
-      <c r="K118" s="13" t="s">
+      <c r="J118" s="13" t="s">
         <v>329</v>
+      </c>
+      <c r="K118" s="4" t="s">
+        <v>303</v>
       </c>
       <c r="L118" s="20">
         <v>20.0</v>
@@ -7613,16 +7621,16 @@
       <c r="I119" s="2">
         <v>87.0</v>
       </c>
-      <c r="J119" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K119" s="13" t="s">
+      <c r="J119" s="13" t="s">
         <v>332</v>
       </c>
-      <c r="L119" s="5">
+      <c r="K119" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L119" s="4">
         <v>300.0</v>
       </c>
-      <c r="M119" s="5">
+      <c r="M119" s="4">
         <v>700.0</v>
       </c>
       <c r="N119" s="2">
@@ -7656,16 +7664,16 @@
       <c r="I120" s="2">
         <v>88.0</v>
       </c>
-      <c r="J120" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K120" s="13" t="s">
+      <c r="J120" s="13" t="s">
         <v>336</v>
       </c>
-      <c r="L120" s="5">
+      <c r="K120" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L120" s="4">
         <v>300.0</v>
       </c>
-      <c r="M120" s="5">
+      <c r="M120" s="4">
         <v>700.0</v>
       </c>
       <c r="N120" s="2">
@@ -7699,16 +7707,16 @@
       <c r="I121" s="2">
         <v>89.0</v>
       </c>
-      <c r="J121" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K121" s="13" t="s">
+      <c r="J121" s="13" t="s">
         <v>338</v>
       </c>
-      <c r="L121" s="5">
+      <c r="K121" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L121" s="4">
         <v>300.0</v>
       </c>
-      <c r="M121" s="5">
+      <c r="M121" s="4">
         <v>700.0</v>
       </c>
       <c r="N121" s="2">
@@ -7742,10 +7750,10 @@
       <c r="I122" s="2">
         <v>102.0</v>
       </c>
-      <c r="J122" s="5" t="s">
+      <c r="J122" s="13" t="s">
         <v>340</v>
       </c>
-      <c r="K122" s="13" t="s">
+      <c r="K122" s="4" t="s">
         <v>341</v>
       </c>
       <c r="L122" s="1">
@@ -7785,11 +7793,11 @@
       <c r="I123" s="2">
         <v>103.0</v>
       </c>
-      <c r="J123" s="5" t="s">
-        <v>340</v>
-      </c>
-      <c r="K123" s="13" t="s">
+      <c r="J123" s="13" t="s">
         <v>344</v>
+      </c>
+      <c r="K123" s="4" t="s">
+        <v>341</v>
       </c>
       <c r="L123" s="1">
         <v>208.0</v>
@@ -7828,11 +7836,11 @@
       <c r="I124" s="2">
         <v>104.0</v>
       </c>
-      <c r="J124" s="5" t="s">
-        <v>340</v>
-      </c>
-      <c r="K124" s="13" t="s">
+      <c r="J124" s="13" t="s">
         <v>346</v>
+      </c>
+      <c r="K124" s="4" t="s">
+        <v>341</v>
       </c>
       <c r="L124" s="1">
         <v>208.0</v>
@@ -7871,16 +7879,16 @@
       <c r="I125" s="2">
         <v>105.0</v>
       </c>
-      <c r="J125" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K125" s="13" t="s">
+      <c r="J125" s="13" t="s">
         <v>348</v>
       </c>
-      <c r="L125" s="5">
+      <c r="K125" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L125" s="4">
         <v>132.0</v>
       </c>
-      <c r="M125" s="5">
+      <c r="M125" s="4">
         <v>172.0</v>
       </c>
       <c r="N125" s="2">
@@ -7901,7 +7909,7 @@
       <c r="S125" s="10">
         <v>0.814</v>
       </c>
-      <c r="T125" s="5" t="s">
+      <c r="T125" s="4" t="s">
         <v>350</v>
       </c>
     </row>
@@ -7914,16 +7922,16 @@
       <c r="I126" s="2">
         <v>106.0</v>
       </c>
-      <c r="J126" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K126" s="13" t="s">
+      <c r="J126" s="13" t="s">
         <v>351</v>
       </c>
-      <c r="L126" s="5">
+      <c r="K126" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L126" s="4">
         <v>146.0</v>
       </c>
-      <c r="M126" s="5">
+      <c r="M126" s="4">
         <v>158.0</v>
       </c>
       <c r="N126" s="2">
@@ -7944,7 +7952,7 @@
       <c r="S126" s="10">
         <v>0.8101</v>
       </c>
-      <c r="T126" s="5" t="s">
+      <c r="T126" s="4" t="s">
         <v>350</v>
       </c>
     </row>
@@ -7957,16 +7965,16 @@
       <c r="I127" s="2">
         <v>116.0</v>
       </c>
-      <c r="J127" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K127" s="13" t="s">
+      <c r="J127" s="13" t="s">
         <v>353</v>
       </c>
-      <c r="L127" s="5">
+      <c r="K127" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L127" s="4">
         <v>50.0</v>
       </c>
-      <c r="M127" s="5">
+      <c r="M127" s="4">
         <v>50.0</v>
       </c>
       <c r="N127" s="2">
@@ -8000,16 +8008,16 @@
       <c r="I128" s="2">
         <v>120.0</v>
       </c>
-      <c r="J128" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="K128" s="13" t="s">
+      <c r="J128" s="13" t="s">
         <v>355</v>
       </c>
-      <c r="L128" s="5">
+      <c r="K128" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="L128" s="4">
         <v>537.0</v>
       </c>
-      <c r="M128" s="5">
+      <c r="M128" s="4">
         <v>537.0</v>
       </c>
       <c r="N128" s="2">
@@ -8043,16 +8051,16 @@
       <c r="I129" s="2">
         <v>126.0</v>
       </c>
-      <c r="J129" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K129" s="13" t="s">
+      <c r="J129" s="13" t="s">
         <v>357</v>
       </c>
-      <c r="L129" s="5">
+      <c r="K129" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L129" s="4">
         <v>50.0</v>
       </c>
-      <c r="M129" s="5">
+      <c r="M129" s="4">
         <v>50.0</v>
       </c>
       <c r="N129" s="2">
@@ -8087,7 +8095,7 @@
       <c r="G130" s="2"/>
       <c r="H130" s="2"/>
       <c r="I130" s="2"/>
-      <c r="K130" s="13" t="s">
+      <c r="J130" s="13" t="s">
         <v>359</v>
       </c>
       <c r="N130" s="2"/>
@@ -8107,7 +8115,7 @@
       <c r="G131" s="2"/>
       <c r="H131" s="2"/>
       <c r="I131" s="2"/>
-      <c r="K131" s="13" t="s">
+      <c r="J131" s="13" t="s">
         <v>360</v>
       </c>
       <c r="N131" s="2"/>
@@ -8127,7 +8135,7 @@
       <c r="G132" s="2"/>
       <c r="H132" s="2"/>
       <c r="I132" s="2"/>
-      <c r="K132" s="13" t="s">
+      <c r="J132" s="13" t="s">
         <v>361</v>
       </c>
       <c r="N132" s="2"/>
@@ -8147,7 +8155,7 @@
       <c r="G133" s="2"/>
       <c r="H133" s="2"/>
       <c r="I133" s="2"/>
-      <c r="K133" s="13" t="s">
+      <c r="J133" s="13" t="s">
         <v>362</v>
       </c>
       <c r="N133" s="2"/>
@@ -8167,7 +8175,7 @@
       <c r="G134" s="1"/>
       <c r="H134" s="1"/>
       <c r="I134" s="1"/>
-      <c r="K134" s="13" t="s">
+      <c r="J134" s="13" t="s">
         <v>363</v>
       </c>
       <c r="N134" s="2"/>
@@ -8187,10 +8195,10 @@
       <c r="G135" s="1"/>
       <c r="H135" s="1"/>
       <c r="I135" s="1"/>
-      <c r="J135" s="22"/>
-      <c r="K135" s="13" t="s">
+      <c r="J135" s="13" t="s">
         <v>364</v>
       </c>
+      <c r="K135" s="22"/>
       <c r="N135" s="2"/>
       <c r="O135" s="2"/>
       <c r="P135" s="10"/>
@@ -8208,10 +8216,10 @@
       <c r="G136" s="1"/>
       <c r="H136" s="1"/>
       <c r="I136" s="1"/>
-      <c r="J136" s="22"/>
-      <c r="K136" s="13" t="s">
+      <c r="J136" s="13" t="s">
         <v>365</v>
       </c>
+      <c r="K136" s="22"/>
       <c r="N136" s="2"/>
       <c r="O136" s="2"/>
       <c r="P136" s="10"/>
@@ -8229,10 +8237,10 @@
       <c r="G137" s="1"/>
       <c r="H137" s="1"/>
       <c r="I137" s="1"/>
-      <c r="J137" s="22"/>
-      <c r="K137" s="13" t="s">
+      <c r="J137" s="13" t="s">
         <v>366</v>
       </c>
+      <c r="K137" s="22"/>
       <c r="N137" s="2"/>
       <c r="O137" s="2"/>
       <c r="P137" s="10"/>
@@ -8250,10 +8258,10 @@
       <c r="G138" s="1"/>
       <c r="H138" s="1"/>
       <c r="I138" s="1"/>
-      <c r="J138" s="22"/>
-      <c r="K138" s="13" t="s">
+      <c r="J138" s="13" t="s">
         <v>367</v>
       </c>
+      <c r="K138" s="22"/>
       <c r="N138" s="2"/>
       <c r="O138" s="2"/>
       <c r="P138" s="10"/>
@@ -8271,10 +8279,10 @@
       <c r="G139" s="1"/>
       <c r="H139" s="1"/>
       <c r="I139" s="1"/>
-      <c r="J139" s="22"/>
-      <c r="K139" s="13" t="s">
+      <c r="J139" s="13" t="s">
         <v>368</v>
       </c>
+      <c r="K139" s="22"/>
       <c r="N139" s="2"/>
       <c r="O139" s="2"/>
       <c r="P139" s="10"/>
@@ -8292,7 +8300,7 @@
       <c r="G140" s="2"/>
       <c r="H140" s="2"/>
       <c r="I140" s="2"/>
-      <c r="K140" s="13" t="s">
+      <c r="J140" s="13" t="s">
         <v>369</v>
       </c>
       <c r="N140" s="2"/>
@@ -8312,7 +8320,7 @@
       <c r="G141" s="2"/>
       <c r="H141" s="2"/>
       <c r="I141" s="2"/>
-      <c r="K141" s="13" t="s">
+      <c r="J141" s="13" t="s">
         <v>370</v>
       </c>
       <c r="N141" s="2"/>
@@ -8332,7 +8340,7 @@
       <c r="G142" s="2"/>
       <c r="H142" s="2"/>
       <c r="I142" s="2"/>
-      <c r="K142" s="13" t="s">
+      <c r="J142" s="13" t="s">
         <v>371</v>
       </c>
       <c r="N142" s="2"/>
@@ -8352,7 +8360,7 @@
       <c r="G143" s="2"/>
       <c r="H143" s="2"/>
       <c r="I143" s="2"/>
-      <c r="K143" s="13" t="s">
+      <c r="J143" s="13" t="s">
         <v>372</v>
       </c>
       <c r="N143" s="2"/>
@@ -8372,7 +8380,7 @@
       <c r="G144" s="2"/>
       <c r="H144" s="2"/>
       <c r="I144" s="2"/>
-      <c r="K144" s="13" t="s">
+      <c r="J144" s="13" t="s">
         <v>373</v>
       </c>
       <c r="N144" s="2"/>
@@ -8392,7 +8400,7 @@
       <c r="G145" s="2"/>
       <c r="H145" s="2"/>
       <c r="I145" s="2"/>
-      <c r="K145" s="13" t="s">
+      <c r="J145" s="13" t="s">
         <v>374</v>
       </c>
       <c r="N145" s="2"/>
@@ -8412,7 +8420,7 @@
       <c r="G146" s="2"/>
       <c r="H146" s="2"/>
       <c r="I146" s="2"/>
-      <c r="K146" s="13" t="s">
+      <c r="J146" s="13" t="s">
         <v>375</v>
       </c>
       <c r="N146" s="2"/>
@@ -8432,7 +8440,7 @@
       <c r="G147" s="2"/>
       <c r="H147" s="2"/>
       <c r="I147" s="2"/>
-      <c r="K147" s="13" t="s">
+      <c r="J147" s="13" t="s">
         <v>376</v>
       </c>
       <c r="N147" s="2"/>
@@ -8452,7 +8460,7 @@
       <c r="G148" s="2"/>
       <c r="H148" s="2"/>
       <c r="I148" s="2"/>
-      <c r="K148" s="13" t="s">
+      <c r="J148" s="13" t="s">
         <v>377</v>
       </c>
       <c r="N148" s="2"/>
@@ -8472,7 +8480,7 @@
       <c r="G149" s="2"/>
       <c r="H149" s="2"/>
       <c r="I149" s="2"/>
-      <c r="K149" s="13" t="s">
+      <c r="J149" s="13" t="s">
         <v>378</v>
       </c>
       <c r="N149" s="2"/>
@@ -8492,7 +8500,7 @@
       <c r="G150" s="2"/>
       <c r="H150" s="2"/>
       <c r="I150" s="2"/>
-      <c r="K150" s="13" t="s">
+      <c r="J150" s="13" t="s">
         <v>379</v>
       </c>
       <c r="N150" s="2"/>
@@ -8512,7 +8520,7 @@
       <c r="G151" s="2"/>
       <c r="H151" s="2"/>
       <c r="I151" s="2"/>
-      <c r="K151" s="13" t="s">
+      <c r="J151" s="13" t="s">
         <v>380</v>
       </c>
       <c r="N151" s="2"/>
@@ -8532,7 +8540,7 @@
       <c r="G152" s="2"/>
       <c r="H152" s="2"/>
       <c r="I152" s="2"/>
-      <c r="K152" s="13" t="s">
+      <c r="J152" s="13" t="s">
         <v>381</v>
       </c>
       <c r="N152" s="2"/>
@@ -8552,7 +8560,7 @@
       <c r="G153" s="2"/>
       <c r="H153" s="2"/>
       <c r="I153" s="2"/>
-      <c r="K153" s="13" t="s">
+      <c r="J153" s="13" t="s">
         <v>382</v>
       </c>
       <c r="N153" s="2"/>
@@ -8572,7 +8580,7 @@
       <c r="G154" s="2"/>
       <c r="H154" s="2"/>
       <c r="I154" s="2"/>
-      <c r="K154" s="13" t="s">
+      <c r="J154" s="13" t="s">
         <v>383</v>
       </c>
       <c r="N154" s="2"/>
@@ -8592,7 +8600,7 @@
       <c r="G155" s="2"/>
       <c r="H155" s="2"/>
       <c r="I155" s="2"/>
-      <c r="K155" s="13" t="s">
+      <c r="J155" s="13" t="s">
         <v>384</v>
       </c>
       <c r="N155" s="2"/>
@@ -8612,7 +8620,7 @@
       <c r="G156" s="2"/>
       <c r="H156" s="2"/>
       <c r="I156" s="2"/>
-      <c r="K156" s="13" t="s">
+      <c r="J156" s="13" t="s">
         <v>385</v>
       </c>
       <c r="N156" s="2"/>

</xml_diff>